<commit_message>
Tests for sending collections report
</commit_message>
<xml_diff>
--- a/processes/collections/results/revenue_report.xlsx
+++ b/processes/collections/results/revenue_report.xlsx
@@ -17,15 +17,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
-    <t>adios</t>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>21/06/2013</t>
   </si>
   <si>
     <t>Invoice Date</t>
   </si>
   <si>
-    <t>Amount</t>
+    <t>c4b230aff0</t>
   </si>
   <si>
     <t>Invoice Number</t>
@@ -34,7 +37,7 @@
     <t>Customer Name</t>
   </si>
   <si>
-    <t>VAT</t>
+    <t>Miguel Angel Canas Vaz</t>
   </si>
   <si>
     <t>VAT Number</t>
@@ -43,7 +46,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>hola</t>
+    <t>VAT</t>
   </si>
 </sst>
 </file>
@@ -1419,33 +1422,45 @@
   <sheetData>
     <row customHeight="1" r="1" ht="12.65" spans="1:1025">
       <c s="1" r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c s="1" r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c s="1" r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c s="1" r="D1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c s="1" r="E1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c s="1" r="F1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="1" r="G1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1025">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed keep_vba param in order to simplify deployment in heroku
</commit_message>
<xml_diff>
--- a/processes/collections/results/revenue_report.xlsx
+++ b/processes/collections/results/revenue_report.xlsx
@@ -382,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr codeName="Hoja1">
+  <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:AMK2"/>
@@ -1476,7 +1476,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr codeName="Hoja2">
+  <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:AMK1"/>
@@ -2526,7 +2526,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr codeName="Hoja3">
+  <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:AMK1"/>

</xml_diff>